<commit_message>
added more test suits
</commit_message>
<xml_diff>
--- a/selenisum-suite/src/main/resources/DriverFiles/ModuleDriver/SafeWay_Modules.xlsx
+++ b/selenisum-suite/src/main/resources/DriverFiles/ModuleDriver/SafeWay_Modules.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Jobs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Run</t>
   </si>
@@ -38,6 +39,18 @@
   </si>
   <si>
     <t>SafeWay_User_Name_Wrong_Information_TC004</t>
+  </si>
+  <si>
+    <t>SafeWay_Jobs1</t>
+  </si>
+  <si>
+    <t>SafeWay_Jobs4</t>
+  </si>
+  <si>
+    <t>SafeWay_Jobs3</t>
+  </si>
+  <si>
+    <t>SafeWay_Jobs2</t>
   </si>
 </sst>
 </file>
@@ -166,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,7 +214,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,14 +489,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added test cases in excel sheet
</commit_message>
<xml_diff>
--- a/selenisum-suite/src/main/resources/DriverFiles/ModuleDriver/SafeWay_Modules.xlsx
+++ b/selenisum-suite/src/main/resources/DriverFiles/ModuleDriver/SafeWay_Modules.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Run</t>
   </si>
@@ -29,18 +29,6 @@
     <t>ON</t>
   </si>
   <si>
-    <t>SafeWay_login_launchApp_TC001</t>
-  </si>
-  <si>
-    <t>SafeWay_Submit_Wrong_Year_TC002</t>
-  </si>
-  <si>
-    <t>SafeWay_Submit_Right_Year_TC003</t>
-  </si>
-  <si>
-    <t>SafeWay_User_Name_Wrong_Information_TC004</t>
-  </si>
-  <si>
     <t>SafeWay_Jobs1</t>
   </si>
   <si>
@@ -51,6 +39,24 @@
   </si>
   <si>
     <t>SafeWay_Jobs2</t>
+  </si>
+  <si>
+    <t>SF_login_launchApp_TC001</t>
+  </si>
+  <si>
+    <t>SF_Sign_In_Wrong_Info_TC002</t>
+  </si>
+  <si>
+    <t>SF_Sign_Up_Wrong_Info_TC003</t>
+  </si>
+  <si>
+    <t>SF_Sign_Up_Don't_Know_Radio_Button_TC004</t>
+  </si>
+  <si>
+    <t>SF_Sign_Up_Form_Information_Fill_Form_TC005</t>
+  </si>
+  <si>
+    <t>SF_Sign_In_TC006</t>
   </si>
 </sst>
 </file>
@@ -88,7 +94,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,14 +117,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,7 +232,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,42 +468,56 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
     </row>
@@ -498,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -523,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -534,7 +566,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -545,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -556,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Selenium New Test Case Steps as coded by Manpreet.
</commit_message>
<xml_diff>
--- a/selenisum-suite/src/main/resources/DriverFiles/ModuleDriver/SafeWay_Modules.xlsx
+++ b/selenisum-suite/src/main/resources/DriverFiles/ModuleDriver/SafeWay_Modules.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="14760" yWindow="280" windowWidth="19880" windowHeight="9740"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Jobs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Run</t>
   </si>
@@ -57,6 +62,9 @@
   </si>
   <si>
     <t>SF_Sign_In_TC006</t>
+  </si>
+  <si>
+    <t>SF_Shopping_Sign_In_TC007</t>
   </si>
 </sst>
 </file>
@@ -80,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,8 +101,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,28 +118,17 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -136,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -197,7 +200,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,7 +235,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,18 +444,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -474,7 +479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -483,7 +488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -492,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>11</v>
@@ -501,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
@@ -510,10 +515,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
@@ -521,8 +524,24 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -534,12 +553,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -561,7 +580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -572,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -583,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -596,5 +615,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>